<commit_message>
Excel file for Table 2.
</commit_message>
<xml_diff>
--- a/Quantitative Variables Assessed in Third-Party Contracts Excel.xlsx
+++ b/Quantitative Variables Assessed in Third-Party Contracts Excel.xlsx
@@ -75,24 +75,23 @@
     <t>Captivity</t>
   </si>
   <si>
-    <t xml:space="preserve"> n   </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Mean/Prop. </t>
   </si>
   <si>
     <t xml:space="preserve"> Quantitative Variables Assessed in Third-Party Contracts </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 represents missing data </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="#"/>
-    <numFmt numFmtId="167" formatCode="#.000"/>
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="#.000"/>
   </numFmts>
-  <fonts count="433">
+  <fonts count="355">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1102,700 +1101,372 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1832,36 +1503,51 @@
       <b/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="timesnewroman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="timesnewroman"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="timesnewroman"/>
     </font>
   </fonts>
@@ -1873,7 +1559,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="317">
+  <borders count="255">
     <border>
       <left/>
       <right/>
@@ -3551,447 +3237,6 @@
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
       <bottom style="double"/>
       <diagonal style="none"/>
     </border>
@@ -4034,6 +3279,20 @@
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
       <bottom style="double"/>
       <diagonal style="none"/>
     </border>
@@ -4048,56 +3307,49 @@
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
-      <bottom style="double"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="thin"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="thin"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="thin"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="double"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="double"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="double"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
       <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="317">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -4755,612 +4007,364 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="241" fillId="0" borderId="165" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="243" fillId="0" borderId="166" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="244" fillId="0" borderId="167" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="241" fillId="0" borderId="165" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="245" fillId="0" borderId="168" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="247" fillId="0" borderId="169" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="248" fillId="0" borderId="170" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="242" fillId="0" borderId="166" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="244" fillId="0" borderId="167" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="245" fillId="0" borderId="168" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="249" fillId="0" borderId="171" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="246" fillId="0" borderId="169" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="250" fillId="0" borderId="172" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="252" fillId="0" borderId="173" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="253" fillId="0" borderId="174" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="247" fillId="0" borderId="170" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="249" fillId="0" borderId="171" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="250" fillId="0" borderId="172" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="254" fillId="0" borderId="175" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="251" fillId="0" borderId="173" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="255" fillId="0" borderId="176" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="257" fillId="0" borderId="177" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="258" fillId="0" borderId="178" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="252" fillId="0" borderId="174" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="254" fillId="0" borderId="175" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="255" fillId="0" borderId="176" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="259" fillId="0" borderId="179" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="256" fillId="0" borderId="177" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="260" fillId="0" borderId="180" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="262" fillId="0" borderId="181" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="263" fillId="0" borderId="182" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="257" fillId="0" borderId="178" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="259" fillId="0" borderId="179" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="260" fillId="0" borderId="180" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="264" fillId="0" borderId="183" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="261" fillId="0" borderId="181" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="265" fillId="0" borderId="184" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="267" fillId="0" borderId="185" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="268" fillId="0" borderId="186" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="262" fillId="0" borderId="182" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="264" fillId="0" borderId="183" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="265" fillId="0" borderId="184" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="269" fillId="0" borderId="187" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="266" fillId="0" borderId="185" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="270" fillId="0" borderId="188" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="272" fillId="0" borderId="189" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="273" fillId="0" borderId="190" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="267" fillId="0" borderId="186" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="269" fillId="0" borderId="187" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="270" fillId="0" borderId="188" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="274" fillId="0" borderId="191" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="271" fillId="0" borderId="189" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="275" fillId="0" borderId="192" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="277" fillId="0" borderId="193" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="278" fillId="0" borderId="194" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="272" fillId="0" borderId="190" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="274" fillId="0" borderId="191" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="275" fillId="0" borderId="192" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="279" fillId="0" borderId="195" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="276" fillId="0" borderId="193" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="280" fillId="0" borderId="196" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="282" fillId="0" borderId="197" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="283" fillId="0" borderId="198" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="277" fillId="0" borderId="194" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="279" fillId="0" borderId="195" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="280" fillId="0" borderId="196" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="284" fillId="0" borderId="199" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="281" fillId="0" borderId="197" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="285" fillId="0" borderId="200" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="287" fillId="0" borderId="201" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="288" fillId="0" borderId="202" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="282" fillId="0" borderId="198" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="284" fillId="0" borderId="199" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="285" fillId="0" borderId="200" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="289" fillId="0" borderId="203" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="286" fillId="0" borderId="201" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="290" fillId="0" borderId="204" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="292" fillId="0" borderId="205" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="293" fillId="0" borderId="206" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="287" fillId="0" borderId="202" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="289" fillId="0" borderId="203" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="290" fillId="0" borderId="204" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="294" fillId="0" borderId="207" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="291" fillId="0" borderId="205" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="295" fillId="0" borderId="208" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="297" fillId="0" borderId="209" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="298" fillId="0" borderId="210" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="292" fillId="0" borderId="206" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="294" fillId="0" borderId="207" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="295" fillId="0" borderId="208" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="299" fillId="0" borderId="211" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="296" fillId="0" borderId="209" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="300" fillId="0" borderId="212" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="302" fillId="0" borderId="213" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="303" fillId="0" borderId="214" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="297" fillId="0" borderId="210" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="299" fillId="0" borderId="211" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="300" fillId="0" borderId="212" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="304" fillId="0" borderId="215" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="301" fillId="0" borderId="213" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="305" fillId="0" borderId="216" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="307" fillId="0" borderId="217" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="308" fillId="0" borderId="218" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="302" fillId="0" borderId="214" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="304" fillId="0" borderId="215" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="305" fillId="0" borderId="216" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="309" fillId="0" borderId="219" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="306" fillId="0" borderId="217" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="310" fillId="0" borderId="220" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="312" fillId="0" borderId="221" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="313" fillId="0" borderId="222" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="307" fillId="0" borderId="218" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="309" fillId="0" borderId="219" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="310" fillId="0" borderId="220" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="314" fillId="0" borderId="223" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="311" fillId="0" borderId="221" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="315" fillId="0" borderId="224" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="317" fillId="0" borderId="225" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="318" fillId="0" borderId="226" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="312" fillId="0" borderId="222" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="314" fillId="0" borderId="223" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="315" fillId="0" borderId="224" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="319" fillId="0" borderId="227" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="316" fillId="0" borderId="225" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="320" fillId="0" borderId="228" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="322" fillId="0" borderId="229" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="323" fillId="0" borderId="230" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="317" fillId="0" borderId="226" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="319" fillId="0" borderId="227" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="320" fillId="0" borderId="228" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="324" fillId="0" borderId="231" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="321" fillId="0" borderId="229" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="325" fillId="0" borderId="232" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="327" fillId="0" borderId="233" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="328" fillId="0" borderId="234" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="322" fillId="0" borderId="230" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="324" fillId="0" borderId="231" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="325" fillId="0" borderId="232" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="329" fillId="0" borderId="235" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="326" fillId="0" borderId="233" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="330" fillId="0" borderId="236" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="332" fillId="0" borderId="237" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="333" fillId="0" borderId="238" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="327" fillId="0" borderId="234" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="329" fillId="0" borderId="235" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="330" fillId="0" borderId="236" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="334" fillId="0" borderId="239" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="331" fillId="0" borderId="237" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="332" fillId="0" borderId="238" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="333" fillId="0" borderId="239" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="334" fillId="0" borderId="240" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="336" fillId="0" borderId="241" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="338" fillId="0" borderId="242" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="340" fillId="0" borderId="243" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="342" fillId="0" borderId="244" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="343" fillId="0" borderId="245" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="335" fillId="0" borderId="240" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="337" fillId="0" borderId="241" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="338" fillId="0" borderId="242" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="344" fillId="0" borderId="246" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="345" fillId="0" borderId="247" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="346" fillId="0" borderId="248" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="339" fillId="0" borderId="243" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="340" fillId="0" borderId="244" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="342" fillId="0" borderId="245" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="343" fillId="0" borderId="246" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="344" fillId="0" borderId="247" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="345" fillId="0" borderId="248" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="347" fillId="0" borderId="249" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="348" fillId="0" borderId="250" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="349" fillId="0" borderId="251" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="350" fillId="0" borderId="252" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="352" fillId="0" borderId="253" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="353" fillId="0" borderId="254" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="354" fillId="0" borderId="255" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="355" fillId="0" borderId="256" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="357" fillId="0" borderId="257" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="358" fillId="0" borderId="258" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="359" fillId="0" borderId="259" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="360" fillId="0" borderId="260" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="362" fillId="0" borderId="261" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="363" fillId="0" borderId="262" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="364" fillId="0" borderId="263" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="365" fillId="0" borderId="264" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="367" fillId="0" borderId="265" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="368" fillId="0" borderId="266" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="369" fillId="0" borderId="267" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="370" fillId="0" borderId="268" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="372" fillId="0" borderId="269" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="373" fillId="0" borderId="270" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="374" fillId="0" borderId="271" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="375" fillId="0" borderId="272" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="377" fillId="0" borderId="273" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="378" fillId="0" borderId="274" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="379" fillId="0" borderId="275" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="380" fillId="0" borderId="276" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="382" fillId="0" borderId="277" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="383" fillId="0" borderId="278" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="384" fillId="0" borderId="279" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="385" fillId="0" borderId="280" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="387" fillId="0" borderId="281" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="388" fillId="0" borderId="282" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="389" fillId="0" borderId="283" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="390" fillId="0" borderId="284" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="392" fillId="0" borderId="285" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="393" fillId="0" borderId="286" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="394" fillId="0" borderId="287" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="395" fillId="0" borderId="288" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="397" fillId="0" borderId="289" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="398" fillId="0" borderId="290" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="399" fillId="0" borderId="291" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="400" fillId="0" borderId="292" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="402" fillId="0" borderId="293" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="403" fillId="0" borderId="294" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="404" fillId="0" borderId="295" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="405" fillId="0" borderId="296" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="407" fillId="0" borderId="297" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="408" fillId="0" borderId="298" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="409" fillId="0" borderId="299" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="410" fillId="0" borderId="300" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="411" fillId="0" borderId="301" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="412" fillId="0" borderId="302" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="413" fillId="0" borderId="303" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="414" fillId="0" borderId="304" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="416" fillId="0" borderId="305" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="418" fillId="0" borderId="306" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="420" fillId="0" borderId="307" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="422" fillId="0" borderId="308" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="424" fillId="0" borderId="309" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="426" fillId="0" borderId="310" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="427" fillId="0" borderId="311" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="428" fillId="0" borderId="312" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="429" fillId="0" borderId="313" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="430" fillId="0" borderId="314" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="431" fillId="0" borderId="315" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="432" fillId="0" borderId="316" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="347" fillId="0" borderId="249" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="348" fillId="0" borderId="250" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="350" fillId="0" borderId="251" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="352" fillId="0" borderId="252" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="353" fillId="0" borderId="253" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="354" fillId="0" borderId="254" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -5372,27 +4376,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:D46"/>
+  <dimension ref="B3:C47"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="3">
-      <c r="B3" s="308" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="308" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="308" t="s">
-        <v>22</v>
+      <c r="B3" s="243" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="243" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="311"/>
-      <c r="C4" s="312" t="s">
+      <c r="B4" s="245"/>
+      <c r="C4" s="246" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" s="313" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -5400,9 +4398,6 @@
         <v>0</v>
       </c>
       <c r="C5" s="108">
-        <v>224</v>
-      </c>
-      <c r="D5" s="170">
         <v>4.2566964285714288</v>
       </c>
     </row>
@@ -5411,9 +4406,6 @@
         <v>1</v>
       </c>
       <c r="C6" s="112">
-        <v>229</v>
-      </c>
-      <c r="D6" s="174">
         <v>0.94759825327510916</v>
       </c>
     </row>
@@ -5422,9 +4414,6 @@
         <v>2</v>
       </c>
       <c r="C7" s="116">
-        <v>229</v>
-      </c>
-      <c r="D7" s="178">
         <v>0.29257641921397382</v>
       </c>
     </row>
@@ -5433,9 +4422,6 @@
         <v>3</v>
       </c>
       <c r="C8" s="120">
-        <v>229</v>
-      </c>
-      <c r="D8" s="182">
         <v>0.27074235807860259</v>
       </c>
     </row>
@@ -5444,9 +4430,6 @@
         <v>4</v>
       </c>
       <c r="C9" s="124">
-        <v>229</v>
-      </c>
-      <c r="D9" s="186">
         <v>0.48908296943231439</v>
       </c>
     </row>
@@ -5455,9 +4438,6 @@
         <v>5</v>
       </c>
       <c r="C10" s="128">
-        <v>229</v>
-      </c>
-      <c r="D10" s="190">
         <v>0.240174672489083</v>
       </c>
     </row>
@@ -5465,15 +4445,12 @@
       <c r="B11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="132">
-        <v>229</v>
-      </c>
     </row>
     <row r="12">
       <c r="B12" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="194">
+      <c r="C12" s="132">
         <v>0.63318777292576423</v>
       </c>
     </row>
@@ -5481,7 +4458,7 @@
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="198">
+      <c r="C13" s="136">
         <v>0.34497816593886471</v>
       </c>
     </row>
@@ -5489,7 +4466,7 @@
       <c r="B14" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="202">
+      <c r="C14" s="140">
         <v>0.021834061135371199</v>
       </c>
     </row>
@@ -5497,15 +4474,12 @@
       <c r="B15" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="136">
-        <v>229</v>
-      </c>
     </row>
     <row r="16">
       <c r="B16" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="206">
+      <c r="C16" s="144">
         <v>0.82969432314410485</v>
       </c>
     </row>
@@ -5513,7 +4487,7 @@
       <c r="B17" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="210">
+      <c r="C17" s="148">
         <v>0.148471615720524</v>
       </c>
     </row>
@@ -5521,7 +4495,7 @@
       <c r="B18" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="214">
+      <c r="C18" s="152">
         <v>0.021834061135371199</v>
       </c>
     </row>
@@ -5529,15 +4503,12 @@
       <c r="B19" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="140">
-        <v>229</v>
-      </c>
     </row>
     <row r="20">
       <c r="B20" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="218">
+      <c r="C20" s="156">
         <v>0.49344978165938858</v>
       </c>
     </row>
@@ -5545,7 +4516,7 @@
       <c r="B21" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="222">
+      <c r="C21" s="160">
         <v>0.48471615720524019</v>
       </c>
     </row>
@@ -5553,7 +4524,7 @@
       <c r="B22" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="226">
+      <c r="C22" s="164">
         <v>0.021834061135371199</v>
       </c>
     </row>
@@ -5561,15 +4532,12 @@
       <c r="B23" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="144">
-        <v>229</v>
-      </c>
     </row>
     <row r="24">
       <c r="B24" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="230">
+      <c r="C24" s="168">
         <v>0.68558951965065507</v>
       </c>
     </row>
@@ -5577,7 +4545,7 @@
       <c r="B25" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="234">
+      <c r="C25" s="172">
         <v>0.28820960698689962</v>
       </c>
     </row>
@@ -5585,7 +4553,7 @@
       <c r="B26" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="238">
+      <c r="C26" s="176">
         <v>0.0262008733624454</v>
       </c>
     </row>
@@ -5593,15 +4561,12 @@
       <c r="B27" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="148">
-        <v>229</v>
-      </c>
     </row>
     <row r="28">
       <c r="B28" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="242">
+      <c r="C28" s="180">
         <v>0.55895196506550215</v>
       </c>
     </row>
@@ -5609,7 +4574,7 @@
       <c r="B29" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="246">
+      <c r="C29" s="184">
         <v>0.42794759825327511</v>
       </c>
     </row>
@@ -5617,7 +4582,7 @@
       <c r="B30" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="250">
+      <c r="C30" s="188">
         <v>0.0131004366812227</v>
       </c>
     </row>
@@ -5625,15 +4590,12 @@
       <c r="B31" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="152">
-        <v>229</v>
-      </c>
     </row>
     <row r="32">
       <c r="B32" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="254">
+      <c r="C32" s="192">
         <v>0.75109170305676853</v>
       </c>
     </row>
@@ -5641,7 +4603,7 @@
       <c r="B33" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="258">
+      <c r="C33" s="196">
         <v>0.23144104803493451</v>
       </c>
     </row>
@@ -5649,7 +4611,7 @@
       <c r="B34" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="262">
+      <c r="C34" s="200">
         <v>0.017467248908296901</v>
       </c>
     </row>
@@ -5657,15 +4619,12 @@
       <c r="B35" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="156">
-        <v>229</v>
-      </c>
     </row>
     <row r="36">
       <c r="B36" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="266">
+      <c r="C36" s="204">
         <v>0.45851528384279477</v>
       </c>
     </row>
@@ -5673,7 +4632,7 @@
       <c r="B37" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="270">
+      <c r="C37" s="208">
         <v>0.1310043668122271</v>
       </c>
     </row>
@@ -5681,7 +4640,7 @@
       <c r="B38" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="274">
+      <c r="C38" s="212">
         <v>0.41048034934497818</v>
       </c>
     </row>
@@ -5689,15 +4648,12 @@
       <c r="B39" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="160">
-        <v>229</v>
-      </c>
     </row>
     <row r="40">
       <c r="B40" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="278">
+      <c r="C40" s="216">
         <v>0.76855895196506552</v>
       </c>
     </row>
@@ -5705,7 +4661,7 @@
       <c r="B41" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="282">
+      <c r="C41" s="220">
         <v>0.2183406113537118</v>
       </c>
     </row>
@@ -5713,7 +4669,7 @@
       <c r="B42" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="286">
+      <c r="C42" s="224">
         <v>0.0131004366812227</v>
       </c>
     </row>
@@ -5721,15 +4677,12 @@
       <c r="B43" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="164">
-        <v>229</v>
-      </c>
     </row>
     <row r="44">
       <c r="B44" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="290">
+      <c r="C44" s="228">
         <v>0.59825327510917026</v>
       </c>
     </row>
@@ -5737,22 +4690,30 @@
       <c r="B45" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="294">
+      <c r="C45" s="232">
         <v>0.38427947598253281</v>
       </c>
     </row>
     <row r="46">
-      <c r="B46" s="314" t="s">
+      <c r="B46" s="247" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="315"/>
-      <c r="D46" s="316">
+      <c r="C46" s="248">
         <v>0.017467248908296901</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" s="253" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="253" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
+  <mergeCells count="2">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B47:C47"/>
   </mergeCells>
 </worksheet>
 </file>
</xml_diff>